<commit_message>
Adding TC_01 and TC_02 manual testCase of Products.
</commit_message>
<xml_diff>
--- a/InvoiceNinja/src/main/resources/ManualTestCaseDoc.xlsx
+++ b/InvoiceNinja/src/main/resources/ManualTestCaseDoc.xlsx
@@ -120,9 +120,6 @@
     <t>Creste new Product page should be display.</t>
   </si>
   <si>
-    <t>6. Click on users and logout.</t>
-  </si>
-  <si>
     <t>https://app.invoiceninja.com/login</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>Jeevitha</t>
+  </si>
+  <si>
+    <t>7. Click on users and logout.</t>
   </si>
 </sst>
 </file>
@@ -257,7 +257,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -317,17 +317,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -336,7 +325,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -353,50 +342,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -671,7 +657,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -696,114 +682,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" ht="28.5" customHeight="1">
       <c r="A11" s="2" t="s">
@@ -883,6 +869,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
     <mergeCell ref="A10:F10"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:F7"/>
@@ -896,12 +888,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -924,10 +910,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -941,118 +927,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="15">
+      <c r="B5" s="13"/>
+      <c r="C5" s="19">
         <v>44234</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="15">
+      <c r="B6" s="13"/>
+      <c r="C6" s="19">
         <v>44234</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="18"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="19"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" ht="21" customHeight="1">
       <c r="A11" s="2" t="s">
@@ -1081,8 +1067,8 @@
       <c r="B12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="16" t="s">
-        <v>31</v>
+      <c r="C12" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>26</v>
@@ -1097,8 +1083,8 @@
       <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>43</v>
+      <c r="C13" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>27</v>
@@ -1114,7 +1100,7 @@
         <v>24</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>28</v>
@@ -1130,7 +1116,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>29</v>
@@ -1143,13 +1129,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -1159,10 +1145,10 @@
         <v>6</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>28</v>
@@ -1171,12 +1157,14 @@
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="5"/>
+      <c r="A18" s="5">
+        <v>7</v>
+      </c>
       <c r="B18" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>26</v>
@@ -1184,282 +1172,282 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="6" t="s">
+    <row r="21" spans="1:6">
+      <c r="A21" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="8" t="s">
+      <c r="B21" s="13"/>
+      <c r="C21" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="6" t="s">
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="6" t="s">
+      <c r="B22" s="13"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7" t="s">
+      <c r="B23" s="13"/>
+      <c r="C23" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="6" t="s">
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="15">
+      <c r="B24" s="13"/>
+      <c r="C24" s="19">
         <v>44234</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="6" t="s">
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="15">
+      <c r="B25" s="13"/>
+      <c r="C25" s="19">
         <v>44234</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="10" t="s">
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="19"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="6" t="s">
+      <c r="B26" s="8"/>
+      <c r="C26" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="18"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="19"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="6" t="s">
+      <c r="B27" s="13"/>
+      <c r="C27" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="18"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="2" t="s">
+      <c r="B28" s="13"/>
+      <c r="C28" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F29" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="5">
-        <v>1</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-    </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="5">
-        <v>2</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>49</v>
+        <v>22</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
     </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="5">
+        <v>6</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="5">
+        <v>7</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:F6"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="C23:F23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:F21"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C9:F9"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:F26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C12" r:id="rId1"/>
     <hyperlink ref="C13" r:id="rId2" display="adityajangam02@gmail.com/Aditya@1"/>
-    <hyperlink ref="C29" r:id="rId3"/>
+    <hyperlink ref="C31" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>